<commit_message>
Arunkumar K: Developer Registration
</commit_message>
<xml_diff>
--- a/TAP_POM_Framework/data/TC001.xlsx
+++ b/TAP_POM_Framework/data/TC001.xlsx
@@ -16,18 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Username</t>
   </si>
   <si>
     <t>PassWord</t>
-  </si>
-  <si>
-    <t>Test Number</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>sys_admin@ltts.com</t>
@@ -75,10 +69,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,43 +410,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>